<commit_message>
a few corrections to the 3d printed files
</commit_message>
<xml_diff>
--- a/V2_files/heat_inserts version/BOM.xlsx
+++ b/V2_files/heat_inserts version/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t xml:space="preserve">It is possible to replace the 3 main LDX-227 Servos with MR996R (or LKY62) but It is recommended to use LDX-227 as they are more powerful and Precise.</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.amazon.com/Reusable-Newlan-Adjustable-Organizer-Management/dp/B081HH5X61/ref=sr_1_3?crid=MQOEL9BTISOW&amp;dib=eyJ2IjoiMSJ9.N9Kq07QH5Nh_hg8e6nG5_sbURQOxYRpYuvQjhkrK4BBmkFQkFwVCkIGD5k6Yne-PNFGVEZIbqH4hzHoFh51yVoMjZxnvzXbEG_w_ksb9Lakz1uEaYXTyNffboVh1ggdXThv-OMe9rpB0WWC78RhGRAF3OVty9qVqTDaDVEPulw1e3_p-Q-bhXRmN3DEusv9vmEAoh6qX_uGN2bNtMCJHvR76W-cD2Kqp5fge7Wb9-Ww.SOvqr7MEl3F8j_oDmJlUP9g-wVMIxvdxp5toBtrauTk&amp;dib_tag=se&amp;keywords=velcro%2Bstraps&amp;qid=1745194925&amp;sprefix=velcro%2Bstr%2Caps%2C138&amp;sr=8-3&amp;th=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">696ZZ Bearing 6mm x 15mm x 5mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/gp/product/B07FW26HD4/</t>
   </si>
   <si>
     <t xml:space="preserve">Extra Tall Female Stackable Header 2x20 (only used if using Hailo Module)</t>
@@ -218,7 +224,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -246,11 +252,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -336,7 +337,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -523,10 +524,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -870,15 +871,26 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B38" s="2" t="s">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>